<commit_message>
Got DB lookup working on test data
</commit_message>
<xml_diff>
--- a/Lookup_Tables.xlsx
+++ b/Lookup_Tables.xlsx
@@ -8,18 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guy/development/avrsnd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29BE982-4589-0145-9A19-7620AD87E6AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2224CC-DBA8-F544-830A-0FDFD8538D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{DD120292-E540-4843-A0F3-C6A293117715}"/>
+    <workbookView xWindow="20" yWindow="480" windowWidth="37920" windowHeight="22460" xr2:uid="{DD120292-E540-4843-A0F3-C6A293117715}"/>
   </bookViews>
   <sheets>
     <sheet name="RMSLookup" sheetId="1" r:id="rId1"/>
     <sheet name="dBALookup" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="AMPLITUDE">#REF!</definedName>
+    <definedName name="CLOCK_FREQ">#REF!</definedName>
+    <definedName name="FREQ">#REF!</definedName>
     <definedName name="P_ZERO">dBALookup!$D$2</definedName>
+    <definedName name="PEAK_VALUE">#REF!</definedName>
+    <definedName name="PHASE_OFFSET">#REF!</definedName>
+    <definedName name="PRESCALER_DATA">#REF!</definedName>
+    <definedName name="PRESCALER_VALUE">#REF!</definedName>
+    <definedName name="SAMPLE_RATE">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C291BDE-19EC-5B40-9DE8-2BB95DEB5D84}">
   <dimension ref="B2:R258"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3381,7 +3389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E90281-845C-474E-9DCF-9E644CC6E714}">
   <dimension ref="B2:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -3460,63 +3468,63 @@
         <v>0.00,</v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" ref="D5:R14" si="0">CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + D$4)/ P_ZERO), 2), ",")</f>
         <v>30.46,</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>36.48,</v>
       </c>
       <c r="F5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>40.00,</v>
       </c>
       <c r="G5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>42.50,</v>
       </c>
       <c r="H5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>44.44,</v>
       </c>
       <c r="I5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>46.02,</v>
       </c>
       <c r="J5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>47.36,</v>
       </c>
       <c r="K5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>48.52,</v>
       </c>
       <c r="L5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>49.54,</v>
       </c>
       <c r="M5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>50.46,</v>
       </c>
       <c r="N5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>51.29,</v>
       </c>
       <c r="O5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>52.04,</v>
       </c>
       <c r="P5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>52.74,</v>
       </c>
       <c r="Q5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>53.38,</v>
       </c>
       <c r="R5" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B5 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>53.98,</v>
       </c>
     </row>
@@ -3525,67 +3533,67 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" ref="C6:C36" si="1">CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + C$4)/ P_ZERO), 2), ",")</f>
         <v>54.54,</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>55.07,</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>55.56,</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>56.03,</v>
       </c>
       <c r="G6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>56.48,</v>
       </c>
       <c r="H6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>56.90,</v>
       </c>
       <c r="I6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>57.31,</v>
       </c>
       <c r="J6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>57.69,</v>
       </c>
       <c r="K6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>58.06,</v>
       </c>
       <c r="L6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>58.42,</v>
       </c>
       <c r="M6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>58.76,</v>
       </c>
       <c r="N6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>59.08,</v>
       </c>
       <c r="O6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>59.40,</v>
       </c>
       <c r="P6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>59.71,</v>
       </c>
       <c r="Q6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>60.00,</v>
       </c>
       <c r="R6" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B6 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>60.28,</v>
       </c>
     </row>
@@ -3594,67 +3602,67 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>60.56,</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>60.83,</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>61.09,</v>
       </c>
       <c r="F7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>61.34,</v>
       </c>
       <c r="G7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>61.58,</v>
       </c>
       <c r="H7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>61.82,</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>62.05,</v>
       </c>
       <c r="J7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>62.28,</v>
       </c>
       <c r="K7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>62.50,</v>
       </c>
       <c r="L7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>62.71,</v>
       </c>
       <c r="M7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>62.92,</v>
       </c>
       <c r="N7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>63.13,</v>
       </c>
       <c r="O7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>63.33,</v>
       </c>
       <c r="P7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>63.52,</v>
       </c>
       <c r="Q7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>63.71,</v>
       </c>
       <c r="R7" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B7 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>63.90,</v>
       </c>
     </row>
@@ -3663,67 +3671,67 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>64.08,</v>
       </c>
       <c r="D8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>64.26,</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>64.44,</v>
       </c>
       <c r="F8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>64.61,</v>
       </c>
       <c r="G8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>64.78,</v>
       </c>
       <c r="H8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>64.94,</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>65.11,</v>
       </c>
       <c r="J8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>65.26,</v>
       </c>
       <c r="K8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>65.42,</v>
       </c>
       <c r="L8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>65.58,</v>
       </c>
       <c r="M8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>65.73,</v>
       </c>
       <c r="N8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>65.87,</v>
       </c>
       <c r="O8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>66.02,</v>
       </c>
       <c r="P8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>66.16,</v>
       </c>
       <c r="Q8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>66.31,</v>
       </c>
       <c r="R8" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B8 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>66.44,</v>
       </c>
     </row>
@@ -3732,67 +3740,67 @@
         <v>4</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>66.58,</v>
       </c>
       <c r="D9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>66.72,</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>66.85,</v>
       </c>
       <c r="F9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>66.98,</v>
       </c>
       <c r="G9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.11,</v>
       </c>
       <c r="H9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.23,</v>
       </c>
       <c r="I9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.36,</v>
       </c>
       <c r="J9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.48,</v>
       </c>
       <c r="K9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.60,</v>
       </c>
       <c r="L9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.72,</v>
       </c>
       <c r="M9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.84,</v>
       </c>
       <c r="N9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>67.96,</v>
       </c>
       <c r="O9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.07,</v>
       </c>
       <c r="P9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.19,</v>
       </c>
       <c r="Q9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.30,</v>
       </c>
       <c r="R9" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B9 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.41,</v>
       </c>
     </row>
@@ -3801,67 +3809,67 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>68.52,</v>
       </c>
       <c r="D10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.63,</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.73,</v>
       </c>
       <c r="F10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.84,</v>
       </c>
       <c r="G10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>68.94,</v>
       </c>
       <c r="H10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.05,</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.15,</v>
       </c>
       <c r="J10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.25,</v>
       </c>
       <c r="K10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.35,</v>
       </c>
       <c r="L10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.45,</v>
       </c>
       <c r="M10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.54,</v>
       </c>
       <c r="N10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.64,</v>
       </c>
       <c r="O10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.73,</v>
       </c>
       <c r="P10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.83,</v>
       </c>
       <c r="Q10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>69.92,</v>
       </c>
       <c r="R10" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B10 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.01,</v>
       </c>
     </row>
@@ -3870,67 +3878,67 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>70.10,</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.19,</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.28,</v>
       </c>
       <c r="F11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.37,</v>
       </c>
       <c r="G11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.46,</v>
       </c>
       <c r="H11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.54,</v>
       </c>
       <c r="I11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.63,</v>
       </c>
       <c r="J11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.71,</v>
       </c>
       <c r="K11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.80,</v>
       </c>
       <c r="L11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.88,</v>
       </c>
       <c r="M11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>70.96,</v>
       </c>
       <c r="N11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.05,</v>
       </c>
       <c r="O11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.13,</v>
       </c>
       <c r="P11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.21,</v>
       </c>
       <c r="Q11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.29,</v>
       </c>
       <c r="R11" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B11 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.36,</v>
       </c>
     </row>
@@ -3939,67 +3947,67 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>71.44,</v>
       </c>
       <c r="D12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.52,</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.60,</v>
       </c>
       <c r="F12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.67,</v>
       </c>
       <c r="G12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.75,</v>
       </c>
       <c r="H12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.82,</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.90,</v>
       </c>
       <c r="J12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>71.97,</v>
       </c>
       <c r="K12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.04,</v>
       </c>
       <c r="L12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.11,</v>
       </c>
       <c r="M12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.18,</v>
       </c>
       <c r="N12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.26,</v>
       </c>
       <c r="O12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.33,</v>
       </c>
       <c r="P12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.40,</v>
       </c>
       <c r="Q12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.46,</v>
       </c>
       <c r="R12" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B12 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.53,</v>
       </c>
     </row>
@@ -4008,67 +4016,67 @@
         <v>8</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>72.60,</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.67,</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.74,</v>
       </c>
       <c r="F13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.80,</v>
       </c>
       <c r="G13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.87,</v>
       </c>
       <c r="H13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>72.93,</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.00,</v>
       </c>
       <c r="J13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.06,</v>
       </c>
       <c r="K13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.13,</v>
       </c>
       <c r="L13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.19,</v>
       </c>
       <c r="M13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.26,</v>
       </c>
       <c r="N13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.32,</v>
       </c>
       <c r="O13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.38,</v>
       </c>
       <c r="P13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.44,</v>
       </c>
       <c r="Q13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.50,</v>
       </c>
       <c r="R13" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B13 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.56,</v>
       </c>
     </row>
@@ -4077,67 +4085,67 @@
         <v>9</v>
       </c>
       <c r="C14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>73.62,</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.68,</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.74,</v>
       </c>
       <c r="F14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.80,</v>
       </c>
       <c r="G14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.86,</v>
       </c>
       <c r="H14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.92,</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>73.98,</v>
       </c>
       <c r="J14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.04,</v>
       </c>
       <c r="K14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.09,</v>
       </c>
       <c r="L14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.15,</v>
       </c>
       <c r="M14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.21,</v>
       </c>
       <c r="N14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.26,</v>
       </c>
       <c r="O14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.32,</v>
       </c>
       <c r="P14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.38,</v>
       </c>
       <c r="Q14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.43,</v>
       </c>
       <c r="R14" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B14 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="0"/>
         <v>74.49,</v>
       </c>
     </row>
@@ -4146,67 +4154,67 @@
         <v>10</v>
       </c>
       <c r="C15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>74.54,</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" ref="D15:R24" si="2">CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + D$4)/ P_ZERO), 2), ",")</f>
         <v>74.59,</v>
       </c>
       <c r="E15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>74.65,</v>
       </c>
       <c r="F15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>74.70,</v>
       </c>
       <c r="G15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>74.75,</v>
       </c>
       <c r="H15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>74.81,</v>
       </c>
       <c r="I15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>74.86,</v>
       </c>
       <c r="J15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>74.91,</v>
       </c>
       <c r="K15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>74.96,</v>
       </c>
       <c r="L15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.02,</v>
       </c>
       <c r="M15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.07,</v>
       </c>
       <c r="N15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.12,</v>
       </c>
       <c r="O15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.17,</v>
       </c>
       <c r="P15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.22,</v>
       </c>
       <c r="Q15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.27,</v>
       </c>
       <c r="R15" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B15 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.32,</v>
       </c>
     </row>
@@ -4215,67 +4223,67 @@
         <v>11</v>
       </c>
       <c r="C16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>75.37,</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.42,</v>
       </c>
       <c r="E16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.47,</v>
       </c>
       <c r="F16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.51,</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.56,</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.61,</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.66,</v>
       </c>
       <c r="J16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.71,</v>
       </c>
       <c r="K16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.75,</v>
       </c>
       <c r="L16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.80,</v>
       </c>
       <c r="M16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.85,</v>
       </c>
       <c r="N16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.89,</v>
       </c>
       <c r="O16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.94,</v>
       </c>
       <c r="P16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>75.99,</v>
       </c>
       <c r="Q16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.03,</v>
       </c>
       <c r="R16" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B16 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.08,</v>
       </c>
     </row>
@@ -4284,67 +4292,67 @@
         <v>12</v>
       </c>
       <c r="C17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>76.12,</v>
       </c>
       <c r="D17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.17,</v>
       </c>
       <c r="E17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.21,</v>
       </c>
       <c r="F17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.26,</v>
       </c>
       <c r="G17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.30,</v>
       </c>
       <c r="H17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.35,</v>
       </c>
       <c r="I17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.39,</v>
       </c>
       <c r="J17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.43,</v>
       </c>
       <c r="K17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.48,</v>
       </c>
       <c r="L17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.52,</v>
       </c>
       <c r="M17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.56,</v>
       </c>
       <c r="N17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.61,</v>
       </c>
       <c r="O17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.65,</v>
       </c>
       <c r="P17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.69,</v>
       </c>
       <c r="Q17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.73,</v>
       </c>
       <c r="R17" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B17 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.78,</v>
       </c>
     </row>
@@ -4353,67 +4361,67 @@
         <v>13</v>
       </c>
       <c r="C18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>76.82,</v>
       </c>
       <c r="D18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.86,</v>
       </c>
       <c r="E18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.90,</v>
       </c>
       <c r="F18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.94,</v>
       </c>
       <c r="G18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>76.98,</v>
       </c>
       <c r="H18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.03,</v>
       </c>
       <c r="I18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.07,</v>
       </c>
       <c r="J18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.11,</v>
       </c>
       <c r="K18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.15,</v>
       </c>
       <c r="L18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.19,</v>
       </c>
       <c r="M18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.23,</v>
       </c>
       <c r="N18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.27,</v>
       </c>
       <c r="O18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.31,</v>
       </c>
       <c r="P18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.35,</v>
       </c>
       <c r="Q18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.38,</v>
       </c>
       <c r="R18" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B18 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.42,</v>
       </c>
     </row>
@@ -4422,67 +4430,67 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>77.46,</v>
       </c>
       <c r="D19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.50,</v>
       </c>
       <c r="E19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.54,</v>
       </c>
       <c r="F19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.58,</v>
       </c>
       <c r="G19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.62,</v>
       </c>
       <c r="H19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.65,</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.69,</v>
       </c>
       <c r="J19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.73,</v>
       </c>
       <c r="K19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.77,</v>
       </c>
       <c r="L19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.80,</v>
       </c>
       <c r="M19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.84,</v>
       </c>
       <c r="N19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.88,</v>
       </c>
       <c r="O19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.92,</v>
       </c>
       <c r="P19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.95,</v>
       </c>
       <c r="Q19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>77.99,</v>
       </c>
       <c r="R19" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B19 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.03,</v>
       </c>
     </row>
@@ -4491,67 +4499,67 @@
         <v>15</v>
       </c>
       <c r="C20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>78.06,</v>
       </c>
       <c r="D20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.10,</v>
       </c>
       <c r="E20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.13,</v>
       </c>
       <c r="F20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.17,</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.21,</v>
       </c>
       <c r="H20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.24,</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.28,</v>
       </c>
       <c r="J20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.31,</v>
       </c>
       <c r="K20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.35,</v>
       </c>
       <c r="L20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.38,</v>
       </c>
       <c r="M20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.42,</v>
       </c>
       <c r="N20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.45,</v>
       </c>
       <c r="O20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.49,</v>
       </c>
       <c r="P20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.52,</v>
       </c>
       <c r="Q20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.55,</v>
       </c>
       <c r="R20" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B20 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.59,</v>
       </c>
     </row>
@@ -4560,67 +4568,67 @@
         <v>16</v>
       </c>
       <c r="C21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>78.62,</v>
       </c>
       <c r="D21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.66,</v>
       </c>
       <c r="E21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.69,</v>
       </c>
       <c r="F21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.72,</v>
       </c>
       <c r="G21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.76,</v>
       </c>
       <c r="H21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.79,</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.82,</v>
       </c>
       <c r="J21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.86,</v>
       </c>
       <c r="K21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.89,</v>
       </c>
       <c r="L21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.92,</v>
       </c>
       <c r="M21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.96,</v>
       </c>
       <c r="N21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>78.99,</v>
       </c>
       <c r="O21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.02,</v>
       </c>
       <c r="P21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.05,</v>
       </c>
       <c r="Q21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.08,</v>
       </c>
       <c r="R21" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B21 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.12,</v>
       </c>
     </row>
@@ -4629,67 +4637,67 @@
         <v>17</v>
       </c>
       <c r="C22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>79.15,</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.18,</v>
       </c>
       <c r="E22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.21,</v>
       </c>
       <c r="F22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.24,</v>
       </c>
       <c r="G22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.28,</v>
       </c>
       <c r="H22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.31,</v>
       </c>
       <c r="I22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.34,</v>
       </c>
       <c r="J22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.37,</v>
       </c>
       <c r="K22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.40,</v>
       </c>
       <c r="L22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.43,</v>
       </c>
       <c r="M22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.46,</v>
       </c>
       <c r="N22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.49,</v>
       </c>
       <c r="O22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.52,</v>
       </c>
       <c r="P22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.55,</v>
       </c>
       <c r="Q22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.58,</v>
       </c>
       <c r="R22" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B22 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.62,</v>
       </c>
     </row>
@@ -4698,67 +4706,67 @@
         <v>18</v>
       </c>
       <c r="C23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>79.65,</v>
       </c>
       <c r="D23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.68,</v>
       </c>
       <c r="E23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.71,</v>
       </c>
       <c r="F23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.74,</v>
       </c>
       <c r="G23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.77,</v>
       </c>
       <c r="H23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.79,</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.82,</v>
       </c>
       <c r="J23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.85,</v>
       </c>
       <c r="K23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.88,</v>
       </c>
       <c r="L23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.91,</v>
       </c>
       <c r="M23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.94,</v>
       </c>
       <c r="N23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>79.97,</v>
       </c>
       <c r="O23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.00,</v>
       </c>
       <c r="P23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.03,</v>
       </c>
       <c r="Q23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.06,</v>
       </c>
       <c r="R23" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B23 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.09,</v>
       </c>
     </row>
@@ -4767,67 +4775,67 @@
         <v>19</v>
       </c>
       <c r="C24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>80.12,</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.14,</v>
       </c>
       <c r="E24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.17,</v>
       </c>
       <c r="F24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.20,</v>
       </c>
       <c r="G24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.23,</v>
       </c>
       <c r="H24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.26,</v>
       </c>
       <c r="I24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.28,</v>
       </c>
       <c r="J24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.31,</v>
       </c>
       <c r="K24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.34,</v>
       </c>
       <c r="L24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.37,</v>
       </c>
       <c r="M24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.40,</v>
       </c>
       <c r="N24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.42,</v>
       </c>
       <c r="O24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.45,</v>
       </c>
       <c r="P24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.48,</v>
       </c>
       <c r="Q24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.51,</v>
       </c>
       <c r="R24" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B24 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="2"/>
         <v>80.53,</v>
       </c>
     </row>
@@ -4836,67 +4844,67 @@
         <v>20</v>
       </c>
       <c r="C25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>80.56,</v>
       </c>
       <c r="D25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" ref="D25:R36" si="3">CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + D$4)/ P_ZERO), 2), ",")</f>
         <v>80.59,</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.61,</v>
       </c>
       <c r="F25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.64,</v>
       </c>
       <c r="G25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.67,</v>
       </c>
       <c r="H25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.70,</v>
       </c>
       <c r="I25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.72,</v>
       </c>
       <c r="J25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.75,</v>
       </c>
       <c r="K25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.78,</v>
       </c>
       <c r="L25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.80,</v>
       </c>
       <c r="M25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.83,</v>
       </c>
       <c r="N25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.85,</v>
       </c>
       <c r="O25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.88,</v>
       </c>
       <c r="P25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.91,</v>
       </c>
       <c r="Q25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.93,</v>
       </c>
       <c r="R25" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B25 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>80.96,</v>
       </c>
     </row>
@@ -4905,67 +4913,67 @@
         <v>21</v>
       </c>
       <c r="C26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>80.98,</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.01,</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.04,</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.06,</v>
       </c>
       <c r="G26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.09,</v>
       </c>
       <c r="H26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.11,</v>
       </c>
       <c r="I26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.14,</v>
       </c>
       <c r="J26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.16,</v>
       </c>
       <c r="K26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.19,</v>
       </c>
       <c r="L26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.21,</v>
       </c>
       <c r="M26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.24,</v>
       </c>
       <c r="N26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.26,</v>
       </c>
       <c r="O26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.29,</v>
       </c>
       <c r="P26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.31,</v>
       </c>
       <c r="Q26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.34,</v>
       </c>
       <c r="R26" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B26 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.36,</v>
       </c>
     </row>
@@ -4974,67 +4982,67 @@
         <v>22</v>
       </c>
       <c r="C27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>81.39,</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.41,</v>
       </c>
       <c r="E27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.44,</v>
       </c>
       <c r="F27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.46,</v>
       </c>
       <c r="G27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.49,</v>
       </c>
       <c r="H27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.51,</v>
       </c>
       <c r="I27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.54,</v>
       </c>
       <c r="J27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.56,</v>
       </c>
       <c r="K27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.58,</v>
       </c>
       <c r="L27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.61,</v>
       </c>
       <c r="M27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.63,</v>
       </c>
       <c r="N27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.66,</v>
       </c>
       <c r="O27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.68,</v>
       </c>
       <c r="P27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.70,</v>
       </c>
       <c r="Q27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.73,</v>
       </c>
       <c r="R27" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B27 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.75,</v>
       </c>
     </row>
@@ -5043,67 +5051,67 @@
         <v>23</v>
       </c>
       <c r="C28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>81.77,</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.80,</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.82,</v>
       </c>
       <c r="F28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.85,</v>
       </c>
       <c r="G28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.87,</v>
       </c>
       <c r="H28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.89,</v>
       </c>
       <c r="I28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.92,</v>
       </c>
       <c r="J28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.94,</v>
       </c>
       <c r="K28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.96,</v>
       </c>
       <c r="L28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>81.98,</v>
       </c>
       <c r="M28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.01,</v>
       </c>
       <c r="N28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.03,</v>
       </c>
       <c r="O28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.05,</v>
       </c>
       <c r="P28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.08,</v>
       </c>
       <c r="Q28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.10,</v>
       </c>
       <c r="R28" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B28 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.12,</v>
       </c>
     </row>
@@ -5112,67 +5120,67 @@
         <v>24</v>
       </c>
       <c r="C29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>82.14,</v>
       </c>
       <c r="D29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.17,</v>
       </c>
       <c r="E29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.19,</v>
       </c>
       <c r="F29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.21,</v>
       </c>
       <c r="G29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.23,</v>
       </c>
       <c r="H29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.26,</v>
       </c>
       <c r="I29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.28,</v>
       </c>
       <c r="J29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.30,</v>
       </c>
       <c r="K29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.32,</v>
       </c>
       <c r="L29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.35,</v>
       </c>
       <c r="M29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.37,</v>
       </c>
       <c r="N29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.39,</v>
       </c>
       <c r="O29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.41,</v>
       </c>
       <c r="P29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.43,</v>
       </c>
       <c r="Q29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.46,</v>
       </c>
       <c r="R29" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B29 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.48,</v>
       </c>
     </row>
@@ -5181,67 +5189,67 @@
         <v>25</v>
       </c>
       <c r="C30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>82.50,</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.52,</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.54,</v>
       </c>
       <c r="F30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.56,</v>
       </c>
       <c r="G30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.59,</v>
       </c>
       <c r="H30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.61,</v>
       </c>
       <c r="I30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.63,</v>
       </c>
       <c r="J30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.65,</v>
       </c>
       <c r="K30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.67,</v>
       </c>
       <c r="L30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.69,</v>
       </c>
       <c r="M30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.71,</v>
       </c>
       <c r="N30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.73,</v>
       </c>
       <c r="O30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.76,</v>
       </c>
       <c r="P30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.78,</v>
       </c>
       <c r="Q30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.80,</v>
       </c>
       <c r="R30" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B30 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.82,</v>
       </c>
     </row>
@@ -5250,67 +5258,67 @@
         <v>26</v>
       </c>
       <c r="C31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>82.84,</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.86,</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.88,</v>
       </c>
       <c r="F31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.90,</v>
       </c>
       <c r="G31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.92,</v>
       </c>
       <c r="H31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.94,</v>
       </c>
       <c r="I31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.96,</v>
       </c>
       <c r="J31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>82.98,</v>
       </c>
       <c r="K31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.00,</v>
       </c>
       <c r="L31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.03,</v>
       </c>
       <c r="M31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.05,</v>
       </c>
       <c r="N31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.07,</v>
       </c>
       <c r="O31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.09,</v>
       </c>
       <c r="P31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.11,</v>
       </c>
       <c r="Q31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.13,</v>
       </c>
       <c r="R31" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B31 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.15,</v>
       </c>
     </row>
@@ -5319,67 +5327,67 @@
         <v>27</v>
       </c>
       <c r="C32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>83.17,</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.19,</v>
       </c>
       <c r="E32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.21,</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.23,</v>
       </c>
       <c r="G32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.25,</v>
       </c>
       <c r="H32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.27,</v>
       </c>
       <c r="I32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.29,</v>
       </c>
       <c r="J32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.31,</v>
       </c>
       <c r="K32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.33,</v>
       </c>
       <c r="L32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.35,</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.37,</v>
       </c>
       <c r="N32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.39,</v>
       </c>
       <c r="O32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.41,</v>
       </c>
       <c r="P32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.42,</v>
       </c>
       <c r="Q32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.44,</v>
       </c>
       <c r="R32" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B32 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.46,</v>
       </c>
     </row>
@@ -5388,67 +5396,67 @@
         <v>28</v>
       </c>
       <c r="C33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>83.48,</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.50,</v>
       </c>
       <c r="E33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.52,</v>
       </c>
       <c r="F33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.54,</v>
       </c>
       <c r="G33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.56,</v>
       </c>
       <c r="H33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.58,</v>
       </c>
       <c r="I33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.60,</v>
       </c>
       <c r="J33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.62,</v>
       </c>
       <c r="K33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.64,</v>
       </c>
       <c r="L33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.66,</v>
       </c>
       <c r="M33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.67,</v>
       </c>
       <c r="N33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.69,</v>
       </c>
       <c r="O33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.71,</v>
       </c>
       <c r="P33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.73,</v>
       </c>
       <c r="Q33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.75,</v>
       </c>
       <c r="R33" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B33 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.77,</v>
       </c>
     </row>
@@ -5457,67 +5465,67 @@
         <v>29</v>
       </c>
       <c r="C34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>83.79,</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.81,</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.83,</v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.84,</v>
       </c>
       <c r="G34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.86,</v>
       </c>
       <c r="H34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.88,</v>
       </c>
       <c r="I34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.90,</v>
       </c>
       <c r="J34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.92,</v>
       </c>
       <c r="K34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.94,</v>
       </c>
       <c r="L34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.95,</v>
       </c>
       <c r="M34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.97,</v>
       </c>
       <c r="N34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>83.99,</v>
       </c>
       <c r="O34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.01,</v>
       </c>
       <c r="P34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.03,</v>
       </c>
       <c r="Q34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.05,</v>
       </c>
       <c r="R34" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B34 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.06,</v>
       </c>
     </row>
@@ -5526,67 +5534,67 @@
         <v>30</v>
       </c>
       <c r="C35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>84.08,</v>
       </c>
       <c r="D35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.10,</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.12,</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.14,</v>
       </c>
       <c r="G35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.15,</v>
       </c>
       <c r="H35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.17,</v>
       </c>
       <c r="I35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.19,</v>
       </c>
       <c r="J35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.21,</v>
       </c>
       <c r="K35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.23,</v>
       </c>
       <c r="L35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.24,</v>
       </c>
       <c r="M35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.26,</v>
       </c>
       <c r="N35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.28,</v>
       </c>
       <c r="O35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.30,</v>
       </c>
       <c r="P35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.31,</v>
       </c>
       <c r="Q35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.33,</v>
       </c>
       <c r="R35" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B35 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.35,</v>
       </c>
     </row>
@@ -5595,67 +5603,67 @@
         <v>31</v>
       </c>
       <c r="C36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + C$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="1"/>
         <v>84.37,</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + D$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.38,</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + E$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.40,</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + F$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.42,</v>
       </c>
       <c r="G36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + G$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.44,</v>
       </c>
       <c r="H36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + H$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.45,</v>
       </c>
       <c r="I36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + I$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.47,</v>
       </c>
       <c r="J36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + J$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.49,</v>
       </c>
       <c r="K36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + K$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.51,</v>
       </c>
       <c r="L36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + L$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.52,</v>
       </c>
       <c r="M36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + M$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.54,</v>
       </c>
       <c r="N36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + N$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.56,</v>
       </c>
       <c r="O36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + O$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.57,</v>
       </c>
       <c r="P36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + P$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.59,</v>
       </c>
       <c r="Q36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + Q$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.61,</v>
       </c>
       <c r="R36" s="3" t="str">
-        <f>CONCATENATE(FIXED(20 *LOG10((($B36 * 16) + R$4)/ P_ZERO), 2), ",")</f>
+        <f t="shared" si="3"/>
         <v>84.63,</v>
       </c>
     </row>

</xml_diff>